<commit_message>
updating code with new functionality
</commit_message>
<xml_diff>
--- a/updated.xlsx
+++ b/updated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Title</t>
   </si>
@@ -25,94 +25,19 @@
     <t>URL</t>
   </si>
   <si>
-    <t xml:space="preserve">Hydronic balancing: is there a better way? In this episode of Taking the Temperature on HVACR, our experts recall the challenge </t>
-  </si>
-  <si>
-    <t>Dorin’s Commitment to a PFAS-free Future in Refrigeration</t>
-  </si>
-  <si>
-    <t>Hanbell Consistently Launches High-efficiency Screw Compressor Models</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What if a #DORIN starter pack looked like this?  What would you still include in the ultimate DORIN sta</t>
-  </si>
-  <si>
-    <t>Our solutions are designed to help you optimize energy efficiency and reduce the development time for both water- and air-cooled</t>
-  </si>
-  <si>
-    <t>Fernwärme-Konferenz fokussiert Fernwärmeausbau</t>
-  </si>
-  <si>
-    <t>Danfoss Thermostatköpfe tauschen leicht gemacht.</t>
-  </si>
-  <si>
-    <t>G&amp;D CHILLERS, INC. has chosen #Frascold Z model #compressors for the new Elite 290 series, developed to provide cutting-edge sol</t>
-  </si>
-  <si>
-    <t>Retrofitting is more than just energy savings. Did you know that by optimizing HVAC systems and energy flows, you can lower oper</t>
-  </si>
-  <si>
-    <t>Danfoss Turbocor: The new Turbocor plant in Tallahassee showcases advanced automation in the manufacturing process</t>
-  </si>
-  <si>
-    <t>Hydronic balancing: is there a better way? In this episode of Taking the Temperature on HVACR, our experts recall the challenge of manually balancing heating systems—adjusting valves, wasting time, and struggling to get it just right. Find out how dynamic balancing solutions can eliminate these inefficiencies, improve comfort, and reduce energy costs in multi-family buildings.  Listen to the full episode now: https://bit.ly/4208oG3#TakingTheTemperatureOnHVACR #HydronicBalancing #MultiFamilyBuildings #</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Officine Mario Dorin is actively addressing the transition away from PFAS in refrigeration.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In response to the growing demand for high-efficiency products, Hanbell launched the RM-Pro series PM VFD screw compressor in 2024.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What if a #DORIN starter pack looked like this? What would you still include in the ultimate DORIN starter kit? Drop it in the comments! At DORIN, we know it takes more than tools – it takes passion, innovation, and a serious love for CO₂You can’t box experience, but you can show what it means to be #Born2Freeze Image created with #AI#trend #artificialintelligence #DORIN #Born2Freeze #since1918 #passion #familybusiness #NatRefs #Innovation #RefrigerationTech #HVACR #CO2cooling #R744 #NaturalRe</t>
-  </si>
-  <si>
-    <t>Our solutions are designed to help you optimize energy efficiency and reduce the development time for both water- and air-cooled systems.  Find all the insights for building better chillers here: https://bit.ly/3WEIIvK#Animation #Chiller #WaterCooled #HVAC</t>
-  </si>
-  <si>
-    <t>Die Expertenvorträge der diesjährigen Danfoss Fernwärme-Konferenz befassen sich mit allen zentralen Herausforderungen der Fernwärmewende – von der Projektplanung über die Dekarbonisierung der Netze durch die Nutzung alternativer Wärmequellen bis zur Optimierung des Netzbetriebs. Praxisbeispiele runden die Vortragsreihe ab. Interessierte haben die Möglichkeit, sich im Rahmen der Online-Veranstaltung vom 20. bis 22. Mai über planerische, technische, rechtliche und wirtschaftliche Aspekte der Umsetzung von Fer</t>
-  </si>
-  <si>
-    <t>Alt gegen Neu: Wir zeigen Ihnen welcher Kopf in welchem Anwendungsfall am besten passt!</t>
-  </si>
-  <si>
-    <t>G&amp;D CHILLERS, INC. has chosen #Frascold Z model #compressors for the new Elite 290 series, developed to provide cutting-edge solutions using #R290. This technology marks a major step forward for the industry, combining #sustainability with high performance.Frascold’s expertise in #NaturalRefrigerant applications played a key role in developing an efficient, low-impact system. Read the full #article to learn more: https://lnkd.in/dnnKbvQ2</t>
-  </si>
-  <si>
-    <t>Retrofitting is more than just energy savings. Did you know that by optimizing HVAC systems and energy flows, you can lower operational expenses while also improving your building’s overall performance?  Danfoss provides retrofit solutions that enhance your building’s efficiency, enabling you to reduce costs and increase long-term value. Let’s work together to retrofit your buildings.  Learn more here: https://bit.ly/4iwG0RO#Retrofit #CommercialBuildings #DanfossClimateSolutions #HVAC</t>
-  </si>
-  <si>
-    <t>The video shows a factory tour of the new Danfoss Turbocor plant in Tallahassee, Florida, showcasing the production process that involves a high level of automation. One of the notable features highlighted is the fully automated end-of-line test that is conducted using the actual refrigerant, emphasizing the advanced technology and precision involved in the manufacturing process at the plant.</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=b01c4e6f8083a16b3a20e34b1e022d0a</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=18debb0f2c3e6e3b7d25430920421a22</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=2cf8c21ed9c2e686e7c686a1b96d0114</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=ce2529ff2b123370a9094c42f798e38e</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=7cd2a445229eb1fda333fb538ee45c25</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=42a2f3609d659ef16f420773548b8751</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=134f480ca759c54bb2a1faab409691f6</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=3be65020d7314f8670ef573adfe20c59</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=679bc7f8f10cd4d4ebd9d1eb9175085d</t>
-  </si>
-  <si>
-    <t>https://my.intelligence2day.com/cc/view/article/?a=C5E7DD06472E34C4B5FD1D452435834B</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>In this video interview, TEON walks us through their T140 dual-stage air-to-water unit, developed with #Frascold #compressors an</t>
+  </si>
+  <si>
+    <t>In this video interview, TEON walks us through their T140 dual-stage air-to-water unit, developed with #Frascold #compressors and #NaturalRefrigerants.Designed to ensure reliable performance in challenging conditions, the system uses #R290 in the low stage and #R600a in the high stage, operating efficiently from -20°C outdoor temperature up to 90°C supply temperature. The configuration also allows for flexible installation and reduced acoustic impact , key factors in modern #HVAC design.Discover how Fra</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7329086445384552448</t>
+  </si>
+  <si>
+    <t>2025-05-16</t>
   </si>
 </sst>
 </file>
@@ -173,12 +98,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Title"/>
     <tableColumn id="2" name="Summary"/>
     <tableColumn id="3" name="URL"/>
+    <tableColumn id="4" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -469,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,133 +411,31 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>